<commit_message>
modifications for summary statistics
</commit_message>
<xml_diff>
--- a/data/typology.xlsx
+++ b/data/typology.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/u1123114/Documents/projects/kinspace/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A6B45DF-2602-894D-96B4-505159F2584C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADD38562-06C1-554E-A9B8-E3B551625BEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19400" activeTab="2" xr2:uid="{25F42487-C902-944F-BB35-F84E493066D3}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19400" activeTab="4" xr2:uid="{25F42487-C902-944F-BB35-F84E493066D3}"/>
   </bookViews>
   <sheets>
     <sheet name="g0" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="229">
   <si>
     <t>Cluster</t>
   </si>
@@ -4255,8 +4255,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2B1DAD8-DE22-664B-98C9-7E8BF2A578A1}">
   <dimension ref="A1:Y19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6438,8 +6438,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67A54662-BFD1-C64E-910E-648277B273D9}">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6670,6 +6670,9 @@
       </c>
       <c r="D8" t="s">
         <v>74</v>
+      </c>
+      <c r="E8" t="s">
+        <v>56</v>
       </c>
       <c r="F8">
         <v>1</v>

</xml_diff>

<commit_message>
updating the pipeline I should do this more regularly
</commit_message>
<xml_diff>
--- a/data/typology.xlsx
+++ b/data/typology.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/u1123114/Documents/projects/kinspace/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADD38562-06C1-554E-A9B8-E3B551625BEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CA83549-0BCB-2B42-84DF-F9261B6DB2DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19400" activeTab="4" xr2:uid="{25F42487-C902-944F-BB35-F84E493066D3}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19400" xr2:uid="{25F42487-C902-944F-BB35-F84E493066D3}"/>
   </bookViews>
   <sheets>
     <sheet name="g0" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,9 @@
     <sheet name="g2" sheetId="5" r:id="rId5"/>
     <sheet name="networks" sheetId="6" r:id="rId6"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">g0!$A$1:$AT$17</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -41,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="233">
   <si>
     <t>Cluster</t>
   </si>
@@ -242,9 +245,6 @@
   </si>
   <si>
     <t>fX mX e// y//</t>
-  </si>
-  <si>
-    <t>Mode Count</t>
   </si>
   <si>
     <t>Brother, Sister, Cousin</t>
@@ -804,6 +804,21 @@
   </si>
   <si>
     <t>D (BD fZD) (fBS mZS) (S fZS mBS) mZD</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>Eskimo</t>
+  </si>
+  <si>
+    <t>Sudanese</t>
+  </si>
+  <si>
+    <t>Crossed-Type</t>
+  </si>
+  <si>
+    <t>Hawaiian</t>
   </si>
 </sst>
 </file>
@@ -1158,156 +1173,162 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BBB3263-AD56-034E-9EEC-6B7D9CD1C261}">
-  <dimension ref="A1:AS17"/>
+  <dimension ref="A1:AT17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="99.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="31.83203125" customWidth="1"/>
+    <col min="3" max="3" width="99.1640625" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="97.6640625" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="99.6640625" customWidth="1"/>
+    <col min="6" max="6" width="31.83203125" customWidth="1"/>
+    <col min="22" max="22" width="6.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="C1" t="s">
         <v>57</v>
       </c>
       <c r="D1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F1" t="s">
-        <v>1</v>
+        <v>228</v>
       </c>
       <c r="G1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" t="s">
         <v>5</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>6</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>7</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>8</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>9</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>10</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>11</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>12</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>13</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>14</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>15</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>16</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>17</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>18</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>19</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>20</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>21</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>22</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>23</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>24</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>25</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>26</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>27</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>28</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>29</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>30</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>31</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>32</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>33</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AN1" t="s">
         <v>34</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AO1" t="s">
         <v>35</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AP1" t="s">
         <v>36</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AQ1" t="s">
         <v>37</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AR1" t="s">
         <v>38</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AS1" t="s">
         <v>39</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AT1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>41</v>
       </c>
@@ -1318,20 +1339,20 @@
         <v>58</v>
       </c>
       <c r="D2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E2" t="str">
         <f xml:space="preserve"> A2&amp;" "&amp;D2</f>
         <v>A (eB eZ) (yB yZ) (FBS FBD FZS FZS MBS MBD MZS MZD)</v>
       </c>
-      <c r="F2">
-        <v>1</v>
+      <c r="F2" t="s">
+        <v>229</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I2">
         <v>2</v>
@@ -1379,19 +1400,19 @@
         <v>2</v>
       </c>
       <c r="X2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Y2">
         <v>3</v>
       </c>
       <c r="Z2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AA2">
         <v>1</v>
       </c>
       <c r="AB2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AC2">
         <v>2</v>
@@ -1439,13 +1460,16 @@
         <v>2</v>
       </c>
       <c r="AR2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AS2">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AT2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>42</v>
       </c>
@@ -1456,20 +1480,20 @@
         <v>59</v>
       </c>
       <c r="D3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E3" t="str">
         <f t="shared" ref="E3:E17" si="0" xml:space="preserve"> A3&amp;" "&amp;D3</f>
         <v>B eB yB eZ yZ  (FBS FBD FZS FZS MBS MBD MZS MZD)</v>
       </c>
-      <c r="F3">
-        <v>1</v>
+      <c r="F3" t="s">
+        <v>229</v>
       </c>
       <c r="G3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I3">
         <v>3</v>
@@ -1517,19 +1541,19 @@
         <v>3</v>
       </c>
       <c r="X3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Y3">
+        <v>4</v>
+      </c>
+      <c r="Z3">
         <v>5</v>
       </c>
-      <c r="Z3">
-        <v>1</v>
-      </c>
       <c r="AA3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AB3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AC3">
         <v>3</v>
@@ -1577,13 +1601,16 @@
         <v>3</v>
       </c>
       <c r="AR3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AS3">
+        <v>4</v>
+      </c>
+      <c r="AT3">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>43</v>
       </c>
@@ -1594,134 +1621,137 @@
         <v>60</v>
       </c>
       <c r="D4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E4" t="str">
         <f t="shared" si="0"/>
         <v>C eB yB eZ yZ  FBS FBD FZS FZS MBS MBD MZS MZD</v>
       </c>
-      <c r="F4">
-        <v>1</v>
+      <c r="F4" t="s">
+        <v>230</v>
       </c>
       <c r="G4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L4">
+        <v>4</v>
+      </c>
+      <c r="M4">
         <v>5</v>
       </c>
-      <c r="M4">
+      <c r="N4">
         <v>6</v>
       </c>
-      <c r="N4">
+      <c r="O4">
         <v>5</v>
       </c>
-      <c r="O4">
+      <c r="P4">
         <v>6</v>
       </c>
-      <c r="P4">
+      <c r="Q4">
         <v>7</v>
       </c>
-      <c r="Q4">
+      <c r="R4">
         <v>8</v>
       </c>
-      <c r="R4">
+      <c r="S4">
         <v>7</v>
       </c>
-      <c r="S4">
+      <c r="T4">
         <v>8</v>
       </c>
-      <c r="T4">
+      <c r="U4">
         <v>9</v>
       </c>
-      <c r="U4">
+      <c r="V4">
         <v>10</v>
       </c>
-      <c r="V4">
+      <c r="W4">
         <v>9</v>
       </c>
-      <c r="W4">
+      <c r="X4">
         <v>10</v>
       </c>
-      <c r="X4">
+      <c r="Y4">
         <v>11</v>
       </c>
-      <c r="Y4">
+      <c r="Z4">
         <v>12</v>
       </c>
-      <c r="Z4">
-        <v>1</v>
-      </c>
       <c r="AA4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AB4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AC4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AD4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AE4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AF4">
+        <v>4</v>
+      </c>
+      <c r="AG4">
         <v>5</v>
       </c>
-      <c r="AG4">
+      <c r="AH4">
         <v>6</v>
       </c>
-      <c r="AH4">
+      <c r="AI4">
         <v>5</v>
       </c>
-      <c r="AI4">
+      <c r="AJ4">
         <v>6</v>
       </c>
-      <c r="AJ4">
+      <c r="AK4">
         <v>7</v>
       </c>
-      <c r="AK4">
+      <c r="AL4">
         <v>8</v>
       </c>
-      <c r="AL4">
+      <c r="AM4">
         <v>7</v>
       </c>
-      <c r="AM4">
+      <c r="AN4">
         <v>8</v>
       </c>
-      <c r="AN4">
+      <c r="AO4">
         <v>9</v>
       </c>
-      <c r="AO4">
+      <c r="AP4">
         <v>10</v>
       </c>
-      <c r="AP4">
+      <c r="AQ4">
         <v>9</v>
       </c>
-      <c r="AQ4">
+      <c r="AR4">
         <v>10</v>
       </c>
-      <c r="AR4">
+      <c r="AS4">
         <v>11</v>
       </c>
-      <c r="AS4">
+      <c r="AT4">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>44</v>
       </c>
@@ -1732,20 +1762,20 @@
         <v>61</v>
       </c>
       <c r="D5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E5" t="str">
         <f t="shared" si="0"/>
         <v>D eB yB eZ yZ (FBS FBS MZS MZD) (FZS FZD MBS MBD)</v>
       </c>
-      <c r="F5">
-        <v>1</v>
+      <c r="F5" t="s">
+        <v>229</v>
       </c>
       <c r="G5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I5">
         <v>3</v>
@@ -1757,7 +1787,7 @@
         <v>3</v>
       </c>
       <c r="L5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M5">
         <v>4</v>
@@ -1781,7 +1811,7 @@
         <v>4</v>
       </c>
       <c r="T5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="U5">
         <v>3</v>
@@ -1793,19 +1823,19 @@
         <v>3</v>
       </c>
       <c r="X5">
+        <v>3</v>
+      </c>
+      <c r="Y5">
         <v>5</v>
       </c>
-      <c r="Y5">
+      <c r="Z5">
         <v>6</v>
       </c>
-      <c r="Z5">
-        <v>1</v>
-      </c>
       <c r="AA5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AB5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AC5">
         <v>3</v>
@@ -1817,7 +1847,7 @@
         <v>3</v>
       </c>
       <c r="AF5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AG5">
         <v>4</v>
@@ -1841,7 +1871,7 @@
         <v>4</v>
       </c>
       <c r="AN5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AO5">
         <v>3</v>
@@ -1853,13 +1883,16 @@
         <v>3</v>
       </c>
       <c r="AR5">
+        <v>3</v>
+      </c>
+      <c r="AS5">
         <v>5</v>
       </c>
-      <c r="AS5">
+      <c r="AT5">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>45</v>
       </c>
@@ -1870,134 +1903,137 @@
         <v>62</v>
       </c>
       <c r="D6" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E6" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">E B Z (FBS FZS MBS MZS) (FBD FZD MBD MZD) </v>
       </c>
-      <c r="F6">
-        <v>1</v>
+      <c r="F6" t="s">
+        <v>229</v>
       </c>
       <c r="G6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="Q6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="R6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="S6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="U6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="V6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="W6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="X6">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="Y6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Z6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AA6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AB6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AC6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AD6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AE6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AF6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AG6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AH6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AI6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AJ6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AK6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AL6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AM6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AN6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AO6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AP6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AQ6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AR6">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="AS6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:45" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="AT6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>46</v>
       </c>
@@ -2008,20 +2044,20 @@
         <v>63</v>
       </c>
       <c r="D7" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E7" t="str">
         <f t="shared" si="0"/>
         <v>F (B Z) (FBS FBD FZS FZS MBS MBD MZS MZD)</v>
       </c>
-      <c r="F7">
-        <v>1</v>
+      <c r="F7" t="s">
+        <v>229</v>
       </c>
       <c r="G7">
         <v>1</v>
       </c>
       <c r="H7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I7">
         <v>2</v>
@@ -2069,7 +2105,7 @@
         <v>2</v>
       </c>
       <c r="X7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Y7">
         <v>1</v>
@@ -2081,7 +2117,7 @@
         <v>1</v>
       </c>
       <c r="AB7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AC7">
         <v>2</v>
@@ -2129,13 +2165,16 @@
         <v>2</v>
       </c>
       <c r="AR7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AS7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AT7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>47</v>
       </c>
@@ -2146,32 +2185,32 @@
         <v>64</v>
       </c>
       <c r="D8" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E8" t="str">
         <f t="shared" si="0"/>
         <v>G (B FBS MZS) (Z FBD MZD) (FZS FZD MBS MBD)</v>
       </c>
-      <c r="F8">
-        <v>1</v>
+      <c r="F8" t="s">
+        <v>231</v>
       </c>
       <c r="G8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H8">
         <v>2</v>
       </c>
       <c r="I8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J8">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L8">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M8">
         <v>4</v>
@@ -2195,43 +2234,43 @@
         <v>4</v>
       </c>
       <c r="T8">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="U8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V8">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="W8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="X8">
         <v>1</v>
       </c>
       <c r="Y8">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Z8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AA8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AB8">
         <v>1</v>
       </c>
       <c r="AC8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AD8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AE8">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AF8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AG8">
         <v>4</v>
@@ -2255,25 +2294,28 @@
         <v>4</v>
       </c>
       <c r="AN8">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="AO8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AP8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AQ8">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AR8">
         <v>3</v>
       </c>
       <c r="AS8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:45" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+      <c r="AT8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>48</v>
       </c>
@@ -2284,134 +2326,137 @@
         <v>65</v>
       </c>
       <c r="D9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E9" t="str">
         <f t="shared" si="0"/>
         <v>H X //</v>
       </c>
-      <c r="F9">
-        <v>1</v>
+      <c r="F9" t="s">
+        <v>232</v>
       </c>
       <c r="G9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H9">
         <v>2</v>
       </c>
       <c r="I9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="X9">
         <v>1</v>
       </c>
       <c r="Y9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Z9">
         <v>2</v>
       </c>
       <c r="AA9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AB9">
         <v>1</v>
       </c>
       <c r="AC9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AD9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AE9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AF9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AG9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AH9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AI9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AJ9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AK9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AL9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AM9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AN9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AO9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AP9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AQ9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AR9">
         <v>2</v>
       </c>
       <c r="AS9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:45" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="AT9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>49</v>
       </c>
@@ -2428,128 +2473,131 @@
         <f t="shared" si="0"/>
         <v>I fX mX e// y//</v>
       </c>
-      <c r="F10">
-        <v>1</v>
+      <c r="F10" t="s">
+        <v>232</v>
       </c>
       <c r="G10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H10">
         <v>2</v>
       </c>
       <c r="I10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J10">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N10">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="O10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="P10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R10">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="S10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="T10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V10">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="W10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="X10">
         <v>1</v>
       </c>
       <c r="Y10">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Z10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AA10">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AB10">
         <v>4</v>
       </c>
       <c r="AC10">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AD10">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AE10">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AF10">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AG10">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AH10">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AI10">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AJ10">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AK10">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AL10">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AM10">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AN10">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AO10">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AP10">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AQ10">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AR10">
         <v>3</v>
       </c>
       <c r="AS10">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:45" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+      <c r="AT10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>50</v>
       </c>
@@ -2557,23 +2605,23 @@
         <v>18</v>
       </c>
       <c r="C11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D11" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E11" t="str">
         <f t="shared" si="0"/>
         <v>J B Z (FBS FBD FZS FZS MBS MBD MZS MZD)</v>
       </c>
-      <c r="F11">
-        <v>1</v>
+      <c r="F11" t="s">
+        <v>229</v>
       </c>
       <c r="G11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H11">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I11">
         <v>3</v>
@@ -2621,19 +2669,19 @@
         <v>3</v>
       </c>
       <c r="X11">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Y11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Z11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AA11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AB11">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AC11">
         <v>3</v>
@@ -2681,13 +2729,16 @@
         <v>3</v>
       </c>
       <c r="AR11">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AS11">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:45" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="AT11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>51</v>
       </c>
@@ -2695,65 +2746,65 @@
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D12" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E12" t="str">
         <f t="shared" si="0"/>
         <v>K (eB FBeS MZeS) (eZ FBeD MZeD) (yB FByS MZyS yZ FByD MZyD) (FZS MBS) (FZD MBD)</v>
       </c>
-      <c r="F12">
-        <v>1</v>
+      <c r="F12" t="s">
+        <v>231</v>
       </c>
       <c r="G12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H12">
         <v>2</v>
       </c>
       <c r="I12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J12">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K12">
         <v>3</v>
       </c>
       <c r="L12">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M12">
+        <v>4</v>
+      </c>
+      <c r="N12">
         <v>5</v>
       </c>
-      <c r="N12">
-        <v>4</v>
-      </c>
       <c r="O12">
+        <v>4</v>
+      </c>
+      <c r="P12">
         <v>5</v>
       </c>
-      <c r="P12">
-        <v>4</v>
-      </c>
       <c r="Q12">
+        <v>4</v>
+      </c>
+      <c r="R12">
         <v>5</v>
       </c>
-      <c r="R12">
-        <v>4</v>
-      </c>
       <c r="S12">
+        <v>4</v>
+      </c>
+      <c r="T12">
         <v>5</v>
       </c>
-      <c r="T12">
-        <v>2</v>
-      </c>
       <c r="U12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V12">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="W12">
         <v>3</v>
@@ -2765,55 +2816,55 @@
         <v>3</v>
       </c>
       <c r="Z12">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AA12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AB12">
         <v>2</v>
       </c>
       <c r="AC12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AD12">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AE12">
         <v>3</v>
       </c>
       <c r="AF12">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AG12">
+        <v>4</v>
+      </c>
+      <c r="AH12">
         <v>5</v>
       </c>
-      <c r="AH12">
-        <v>4</v>
-      </c>
       <c r="AI12">
+        <v>4</v>
+      </c>
+      <c r="AJ12">
         <v>5</v>
       </c>
-      <c r="AJ12">
-        <v>4</v>
-      </c>
       <c r="AK12">
+        <v>4</v>
+      </c>
+      <c r="AL12">
         <v>5</v>
       </c>
-      <c r="AL12">
-        <v>4</v>
-      </c>
       <c r="AM12">
+        <v>4</v>
+      </c>
+      <c r="AN12">
         <v>5</v>
       </c>
-      <c r="AN12">
-        <v>2</v>
-      </c>
       <c r="AO12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AP12">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AQ12">
         <v>3</v>
@@ -2824,8 +2875,11 @@
       <c r="AS12">
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AT12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>52</v>
       </c>
@@ -2833,23 +2887,23 @@
         <v>4</v>
       </c>
       <c r="C13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D13" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E13" t="str">
         <f t="shared" si="0"/>
         <v>L fX mX (FBS FBD FZS FZS MBS MBD MZS MZD)</v>
       </c>
-      <c r="F13">
-        <v>1</v>
+      <c r="F13" t="s">
+        <v>229</v>
       </c>
       <c r="G13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H13">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I13">
         <v>3</v>
@@ -2897,20 +2951,20 @@
         <v>3</v>
       </c>
       <c r="X13">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Y13">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="Z13">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AA13">
+        <v>2</v>
+      </c>
+      <c r="AB13">
         <v>5</v>
       </c>
-      <c r="AB13">
-        <v>3</v>
-      </c>
       <c r="AC13">
         <v>3</v>
       </c>
@@ -2957,13 +3011,16 @@
         <v>3</v>
       </c>
       <c r="AR13">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AS13">
+        <v>4</v>
+      </c>
+      <c r="AT13">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>53</v>
       </c>
@@ -2971,137 +3028,140 @@
         <v>12</v>
       </c>
       <c r="C14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D14" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E14" t="str">
         <f t="shared" si="0"/>
         <v>M eB yB eZ yZ  e(FBS FBD FZS FZS MBS MBD MZS MZD)  y(FBS FBD FZS FZS MBS MBD MZS MZD)</v>
       </c>
-      <c r="F14">
-        <v>1</v>
+      <c r="F14" t="s">
+        <v>229</v>
       </c>
       <c r="G14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H14">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I14">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J14">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K14">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L14">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M14">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N14">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O14">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P14">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="Q14">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="R14">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="S14">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T14">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="U14">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="V14">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="W14">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="X14">
+        <v>4</v>
+      </c>
+      <c r="Y14">
         <v>5</v>
       </c>
-      <c r="Y14">
+      <c r="Z14">
         <v>6</v>
       </c>
-      <c r="Z14">
-        <v>1</v>
-      </c>
       <c r="AA14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AB14">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AC14">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AD14">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AE14">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AF14">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AG14">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AH14">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AI14">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AJ14">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AK14">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AL14">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AM14">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AN14">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AO14">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AP14">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AQ14">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AR14">
+        <v>4</v>
+      </c>
+      <c r="AS14">
         <v>5</v>
       </c>
-      <c r="AS14">
+      <c r="AT14">
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>54</v>
       </c>
@@ -3109,23 +3169,23 @@
         <v>10</v>
       </c>
       <c r="C15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D15" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E15" t="str">
         <f t="shared" si="0"/>
         <v>N eB eZ (yB yZ)  (FBS FBD FZS FZS MBS MBD MZS MZD)</v>
       </c>
-      <c r="F15">
-        <v>1</v>
+      <c r="F15" t="s">
+        <v>229</v>
       </c>
       <c r="G15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H15">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I15">
         <v>3</v>
@@ -3173,19 +3233,19 @@
         <v>3</v>
       </c>
       <c r="X15">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Y15">
         <v>4</v>
       </c>
       <c r="Z15">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="AA15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AB15">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AC15">
         <v>3</v>
@@ -3233,13 +3293,16 @@
         <v>3</v>
       </c>
       <c r="AR15">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AS15">
         <v>4</v>
       </c>
-    </row>
-    <row r="16" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AT15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>55</v>
       </c>
@@ -3247,137 +3310,140 @@
         <v>3</v>
       </c>
       <c r="C16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D16" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E16" t="str">
         <f t="shared" si="0"/>
         <v>O (eB FBeS FZeS MBeS MZeS) (eD FBeD FZeD MBeD MZeD) (yB FByS FZyS MByS MZyS) (yD FByD FZyD MByD MZyD)</v>
       </c>
-      <c r="F16">
-        <v>1</v>
+      <c r="F16" t="s">
+        <v>231</v>
       </c>
       <c r="G16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H16">
         <v>2</v>
       </c>
       <c r="I16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J16">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K16">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L16">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N16">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="O16">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P16">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="Q16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R16">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="S16">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T16">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="U16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V16">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="W16">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="X16">
         <v>4</v>
       </c>
       <c r="Y16">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="Z16">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AA16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AB16">
         <v>2</v>
       </c>
       <c r="AC16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AD16">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AE16">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AF16">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AG16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AH16">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AI16">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AJ16">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AK16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AL16">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AM16">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AN16">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AO16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AP16">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AQ16">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AR16">
         <v>4</v>
       </c>
       <c r="AS16">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:45" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+      <c r="AT16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>56</v>
       </c>
@@ -3385,15 +3451,12 @@
         <v>5</v>
       </c>
       <c r="C17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E17" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">Outlier </v>
       </c>
-      <c r="F17">
-        <v>1</v>
-      </c>
       <c r="G17">
         <v>1</v>
       </c>
@@ -3404,43 +3467,43 @@
         <v>1</v>
       </c>
       <c r="J17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K17">
         <v>2</v>
       </c>
       <c r="L17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M17">
         <v>1</v>
       </c>
       <c r="N17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O17">
         <v>2</v>
       </c>
       <c r="P17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q17">
         <v>1</v>
       </c>
       <c r="R17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S17">
         <v>2</v>
       </c>
       <c r="T17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U17">
         <v>1</v>
       </c>
       <c r="V17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W17">
         <v>2</v>
@@ -3452,7 +3515,7 @@
         <v>2</v>
       </c>
       <c r="Z17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AA17">
         <v>1</v>
@@ -3464,43 +3527,43 @@
         <v>1</v>
       </c>
       <c r="AD17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AE17">
         <v>2</v>
       </c>
       <c r="AF17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AG17">
         <v>1</v>
       </c>
       <c r="AH17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AI17">
         <v>2</v>
       </c>
       <c r="AJ17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AK17">
         <v>1</v>
       </c>
       <c r="AL17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AM17">
         <v>2</v>
       </c>
       <c r="AN17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AO17">
         <v>1</v>
       </c>
       <c r="AP17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AQ17">
         <v>2</v>
@@ -3511,8 +3574,12 @@
       <c r="AS17">
         <v>2</v>
       </c>
+      <c r="AT17">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:AT17" xr:uid="{0BBB3263-AD56-034E-9EEC-6B7D9CD1C261}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3522,7 +3589,7 @@
   <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E16"/>
+      <selection sqref="A1:E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3538,16 +3605,16 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C1" t="s">
         <v>57</v>
       </c>
       <c r="D1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F1" t="s">
         <v>1</v>
@@ -3582,10 +3649,10 @@
         <v>191</v>
       </c>
       <c r="C2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E2" t="str">
         <f xml:space="preserve"> A2&amp;" "&amp;D2</f>
@@ -3624,10 +3691,10 @@
         <v>107</v>
       </c>
       <c r="C3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E3" t="str">
         <f t="shared" ref="E3:E17" si="0" xml:space="preserve"> A3&amp;" "&amp;D3</f>
@@ -3666,10 +3733,10 @@
         <v>91</v>
       </c>
       <c r="C4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E4" t="str">
         <f t="shared" si="0"/>
@@ -3708,10 +3775,10 @@
         <v>80</v>
       </c>
       <c r="C5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E5" t="str">
         <f t="shared" si="0"/>
@@ -3750,10 +3817,10 @@
         <v>45</v>
       </c>
       <c r="C6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E6" t="str">
         <f t="shared" si="0"/>
@@ -3792,10 +3859,10 @@
         <v>40</v>
       </c>
       <c r="C7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E7" t="str">
         <f t="shared" si="0"/>
@@ -3834,10 +3901,10 @@
         <v>44</v>
       </c>
       <c r="C8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E8" t="str">
         <f t="shared" si="0"/>
@@ -3876,10 +3943,10 @@
         <v>23</v>
       </c>
       <c r="C9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D9" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E9" t="str">
         <f t="shared" si="0"/>
@@ -3918,10 +3985,10 @@
         <v>21</v>
       </c>
       <c r="C10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E10" t="str">
         <f t="shared" si="0"/>
@@ -3960,10 +4027,10 @@
         <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E11" t="str">
         <f t="shared" si="0"/>
@@ -4002,10 +4069,10 @@
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E12" t="str">
         <f t="shared" si="0"/>
@@ -4044,10 +4111,10 @@
         <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E13" t="str">
         <f t="shared" si="0"/>
@@ -4086,10 +4153,10 @@
         <v>11</v>
       </c>
       <c r="C14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D14" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E14" t="str">
         <f t="shared" si="0"/>
@@ -4128,10 +4195,10 @@
         <v>11</v>
       </c>
       <c r="C15" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D15" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E15" t="str">
         <f t="shared" si="0"/>
@@ -4170,10 +4237,10 @@
         <v>9</v>
       </c>
       <c r="C16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D16" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E16" t="str">
         <f t="shared" si="0"/>
@@ -4212,10 +4279,10 @@
         <v>7</v>
       </c>
       <c r="C17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E17" t="str">
         <f t="shared" si="0"/>
@@ -4272,76 +4339,76 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F1" t="s">
+        <v>90</v>
+      </c>
+      <c r="G1" t="s">
         <v>91</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>92</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>93</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>94</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>95</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>96</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>97</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>98</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>99</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>100</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>101</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>102</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>103</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>104</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>105</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>106</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>107</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>108</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>109</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.2">
@@ -4352,10 +4419,10 @@
         <v>93</v>
       </c>
       <c r="C2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E2" t="str">
         <f xml:space="preserve"> A2&amp;" "&amp;D2</f>
@@ -4430,10 +4497,10 @@
         <v>70</v>
       </c>
       <c r="C3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E3" t="str">
         <f t="shared" ref="E3:E19" si="0" xml:space="preserve"> A3&amp;" "&amp;D3</f>
@@ -4508,10 +4575,10 @@
         <v>38</v>
       </c>
       <c r="C4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E4" t="str">
         <f t="shared" si="0"/>
@@ -4586,10 +4653,10 @@
         <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E5" t="str">
         <f t="shared" si="0"/>
@@ -4664,10 +4731,10 @@
         <v>34</v>
       </c>
       <c r="C6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D6" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E6" t="str">
         <f t="shared" si="0"/>
@@ -4742,10 +4809,10 @@
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D7" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E7" t="str">
         <f t="shared" si="0"/>
@@ -4820,10 +4887,10 @@
         <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D8" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E8" t="str">
         <f t="shared" si="0"/>
@@ -4898,7 +4965,7 @@
         <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D9" t="s">
         <v>43</v>
@@ -4976,10 +5043,10 @@
         <v>18</v>
       </c>
       <c r="C10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D10" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E10" t="str">
         <f t="shared" si="0"/>
@@ -5054,10 +5121,10 @@
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D11" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E11" t="str">
         <f t="shared" si="0"/>
@@ -5132,10 +5199,10 @@
         <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D12" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E12" t="str">
         <f t="shared" si="0"/>
@@ -5210,10 +5277,10 @@
         <v>6</v>
       </c>
       <c r="C13" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D13" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E13" t="str">
         <f t="shared" si="0"/>
@@ -5288,10 +5355,10 @@
         <v>5</v>
       </c>
       <c r="C14" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D14" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E14" t="str">
         <f t="shared" si="0"/>
@@ -5366,10 +5433,10 @@
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D15" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E15" t="str">
         <f t="shared" si="0"/>
@@ -5444,10 +5511,10 @@
         <v>13</v>
       </c>
       <c r="C16" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D16" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E16" t="str">
         <f t="shared" si="0"/>
@@ -5516,16 +5583,16 @@
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B17">
         <v>5</v>
       </c>
       <c r="C17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D17" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E17" t="str">
         <f t="shared" si="0"/>
@@ -5594,16 +5661,16 @@
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B18">
         <v>4</v>
       </c>
       <c r="C18" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D18" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E18" t="str">
         <f t="shared" si="0"/>
@@ -5678,7 +5745,7 @@
         <v>4</v>
       </c>
       <c r="C19" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E19" t="str">
         <f t="shared" si="0"/>
@@ -5769,46 +5836,46 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C1" t="s">
         <v>57</v>
       </c>
       <c r="D1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F1" t="s">
+        <v>130</v>
+      </c>
+      <c r="G1" t="s">
         <v>131</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>132</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>133</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>134</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>135</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>136</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>137</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>138</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>139</v>
-      </c>
-      <c r="O1" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
@@ -5819,10 +5886,10 @@
         <v>166</v>
       </c>
       <c r="C2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E2" t="str">
         <f xml:space="preserve"> A2&amp;" "&amp;D2</f>
@@ -5867,10 +5934,10 @@
         <v>131</v>
       </c>
       <c r="C3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E3" t="str">
         <f t="shared" ref="E3:E14" si="0" xml:space="preserve"> A3&amp;" "&amp;D3</f>
@@ -5915,10 +5982,10 @@
         <v>100</v>
       </c>
       <c r="C4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E4" t="str">
         <f t="shared" si="0"/>
@@ -5963,10 +6030,10 @@
         <v>37</v>
       </c>
       <c r="C5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E5" t="str">
         <f t="shared" si="0"/>
@@ -6011,10 +6078,10 @@
         <v>26</v>
       </c>
       <c r="C6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E6" t="str">
         <f t="shared" si="0"/>
@@ -6059,10 +6126,10 @@
         <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D7" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E7" t="str">
         <f t="shared" si="0"/>
@@ -6107,10 +6174,10 @@
         <v>27</v>
       </c>
       <c r="C8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E8" t="str">
         <f t="shared" si="0"/>
@@ -6155,10 +6222,10 @@
         <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D9" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E9" t="str">
         <f t="shared" si="0"/>
@@ -6203,10 +6270,10 @@
         <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D10" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E10" t="str">
         <f t="shared" si="0"/>
@@ -6251,10 +6318,10 @@
         <v>16</v>
       </c>
       <c r="C11" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D11" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E11" t="str">
         <f t="shared" si="0"/>
@@ -6299,10 +6366,10 @@
         <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D12" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E12" t="str">
         <f t="shared" si="0"/>
@@ -6347,10 +6414,10 @@
         <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D13" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E13" t="str">
         <f t="shared" si="0"/>
@@ -6438,7 +6505,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67A54662-BFD1-C64E-910E-648277B273D9}">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
@@ -6454,28 +6521,28 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C1" t="s">
         <v>57</v>
       </c>
       <c r="D1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F1" t="s">
+        <v>152</v>
+      </c>
+      <c r="G1" t="s">
         <v>153</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>154</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>155</v>
-      </c>
-      <c r="I1" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -6486,10 +6553,10 @@
         <v>461</v>
       </c>
       <c r="C2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E2" t="str">
         <f xml:space="preserve"> A2&amp;" "&amp;D2</f>
@@ -6516,10 +6583,10 @@
         <v>213</v>
       </c>
       <c r="C3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E3" t="str">
         <f t="shared" ref="E3:E8" si="0" xml:space="preserve"> A3&amp;" "&amp;D3</f>
@@ -6546,10 +6613,10 @@
         <v>102</v>
       </c>
       <c r="C4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E4" t="str">
         <f t="shared" si="0"/>
@@ -6576,10 +6643,10 @@
         <v>23</v>
       </c>
       <c r="C5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E5" t="str">
         <f t="shared" si="0"/>
@@ -6606,10 +6673,10 @@
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D6" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E6" t="str">
         <f t="shared" si="0"/>
@@ -6636,10 +6703,10 @@
         <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D7" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E7" t="str">
         <f t="shared" si="0"/>
@@ -6666,10 +6733,10 @@
         <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E8" t="s">
         <v>56</v>
@@ -6707,41 +6774,41 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B1" t="s">
         <v>162</v>
-      </c>
-      <c r="B1" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>

</xml_diff>